<commit_message>
Funcionality to add all data to one spreadsheet.
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -8,9 +8,76 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+  <si>
+    <t>Overall Score</t>
+  </si>
+  <si>
+    <t>Productivity</t>
+  </si>
+  <si>
+    <t>Creativity</t>
+  </si>
+  <si>
+    <t>Responsiveness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1685
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1663
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1736
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1603
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1689
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1675
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1719
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1641
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1681
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1664
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1701
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1669
+</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -340,12 +407,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed a bug where importing openpyxl caused errors
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -11,39 +11,6 @@
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Overall Score</t>
-  </si>
-  <si>
-    <t>Productivity</t>
-  </si>
-  <si>
-    <t>Creativity</t>
-  </si>
-  <si>
-    <t>Responsiveness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1726
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1614
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1914
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1549
-</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -373,48 +340,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added xlsx files to gitignore
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -8,9 +8,100 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+  <si>
+    <t>Overall Score</t>
+  </si>
+  <si>
+    <t>Productivity</t>
+  </si>
+  <si>
+    <t>Creativity</t>
+  </si>
+  <si>
+    <t>Responsiveness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1726
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1614
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1914
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1549
+</t>
+  </si>
+  <si>
+    <t>6223</t>
+  </si>
+  <si>
+    <t>Essentials</t>
+  </si>
+  <si>
+    <t>11101</t>
+  </si>
+  <si>
+    <t>Digital Content Creation</t>
+  </si>
+  <si>
+    <t>10373</t>
+  </si>
+  <si>
+    <t>App Startup</t>
+  </si>
+  <si>
+    <t>Video Conferencing</t>
+  </si>
+  <si>
+    <t>5681</t>
+  </si>
+  <si>
+    <t>Web Browsing</t>
+  </si>
+  <si>
+    <t>Spreadsheets</t>
+  </si>
+  <si>
+    <t>17516</t>
+  </si>
+  <si>
+    <t>Writing</t>
+  </si>
+  <si>
+    <t>8168</t>
+  </si>
+  <si>
+    <t>Photo Editing</t>
+  </si>
+  <si>
+    <t>9564</t>
+  </si>
+  <si>
+    <t>Render and Visual</t>
+  </si>
+  <si>
+    <t>11977</t>
+  </si>
+  <si>
+    <t>Video Editing</t>
+  </si>
+  <si>
+    <t>8984</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -340,12 +431,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added buttons to geekbench
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -8,100 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
-  <si>
-    <t>Overall Score</t>
-  </si>
-  <si>
-    <t>Productivity</t>
-  </si>
-  <si>
-    <t>Creativity</t>
-  </si>
-  <si>
-    <t>Responsiveness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1726
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1614
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1914
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1549
-</t>
-  </si>
-  <si>
-    <t>6223</t>
-  </si>
-  <si>
-    <t>Essentials</t>
-  </si>
-  <si>
-    <t>11101</t>
-  </si>
-  <si>
-    <t>Digital Content Creation</t>
-  </si>
-  <si>
-    <t>10373</t>
-  </si>
-  <si>
-    <t>App Startup</t>
-  </si>
-  <si>
-    <t>Video Conferencing</t>
-  </si>
-  <si>
-    <t>5681</t>
-  </si>
-  <si>
-    <t>Web Browsing</t>
-  </si>
-  <si>
-    <t>Spreadsheets</t>
-  </si>
-  <si>
-    <t>17516</t>
-  </si>
-  <si>
-    <t>Writing</t>
-  </si>
-  <si>
-    <t>8168</t>
-  </si>
-  <si>
-    <t>Photo Editing</t>
-  </si>
-  <si>
-    <t>9564</t>
-  </si>
-  <si>
-    <t>Render and Visual</t>
-  </si>
-  <si>
-    <t>11977</t>
-  </si>
-  <si>
-    <t>Video Editing</t>
-  </si>
-  <si>
-    <t>8984</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -431,160 +340,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>